<commit_message>
close #187: Remove unnecessary column name in values ​​and proportionality
</commit_message>
<xml_diff>
--- a/input_data/data_errors_01/proporcionalidades.xlsx
+++ b/input_data/data_errors_01/proporcionalidades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t xml:space="preserve">5008-2010</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">nome</t>
-  </si>
-  <si>
     <t xml:space="preserve">5021-2010</t>
   </si>
   <si>
@@ -70,22 +67,10 @@
     <t xml:space="preserve">5031-2010</t>
   </si>
   <si>
-    <t xml:space="preserve">Alta Floresta</t>
-  </si>
-  <si>
     <t xml:space="preserve">DI</t>
   </si>
   <si>
-    <t xml:space="preserve">Ariquemes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cacoal</t>
-  </si>
-  <si>
     <t xml:space="preserve">PHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cerejeiras</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
@@ -306,39 +291,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="3" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="9.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -377,48 +360,42 @@
       <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1100015</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
+      <c r="B3" s="1" t="n">
+        <v>0.99</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.99</v>
+        <v>0.347</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.347</v>
+        <v>0.211</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>0.211</v>
-      </c>
-      <c r="F3" s="1" t="n">
         <v>0.442</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.558</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0.558</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.1</v>
+        <v>0.098</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="M3" s="1" t="n">
         <v>0.164</v>
       </c>
     </row>
@@ -426,40 +403,37 @@
       <c r="A4" s="1" t="n">
         <v>1100023</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
+      <c r="B4" s="1" t="n">
+        <v>0.441</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0.441</v>
+        <v>0.347</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.347</v>
+        <v>0.211</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>0.211</v>
-      </c>
-      <c r="F4" s="1" t="n">
         <v>0.442</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.558</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0.558</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0</v>
+        <v>0.50699999</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.50699999</v>
+        <v>0.232</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.232</v>
+        <v>0.098</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="M4" s="1" t="n">
         <v>0.164</v>
       </c>
     </row>
@@ -467,40 +441,37 @@
       <c r="A5" s="1" t="n">
         <v>1100049</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
+      <c r="B5" s="1" t="n">
+        <v>0.443</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0.443</v>
+        <v>0.347</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0.347</v>
+        <v>0.211</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>0.211</v>
-      </c>
-      <c r="F5" s="1" t="n">
         <v>0.442</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0.558</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0.558</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>0</v>
+        <v>0.506</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="K5" s="1" t="n">
         <v>0.232</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="1" t="n">
+      <c r="K5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="1" t="n">
         <v>0.164</v>
       </c>
     </row>
@@ -508,40 +479,37 @@
       <c r="A6" s="1" t="n">
         <v>1100056</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
+      <c r="B6" s="1" t="n">
+        <v>0.442</v>
       </c>
       <c r="C6" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="E6" s="1" t="n">
         <v>0.442</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>0.347</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0.211</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="1" t="n">
-        <v>0.558</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="1" t="n">
+      <c r="L6" s="1" t="n">
         <v>0.164</v>
       </c>
     </row>

</xml_diff>